<commit_message>
Audit Table Creation + Timestamp for schema
Adding Audit Timestamp to v1 of schema
Starting adding the synthetic data
</commit_message>
<xml_diff>
--- a/Quality-Schema.xlsx
+++ b/Quality-Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VICTUS\Documents\GitHub\sql-quality-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D92943-D61F-44EE-A886-3968D0DA6AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54073D9B-14C3-457A-9C05-C55EA7BBF2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Type</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>Audit Table</t>
+  </si>
+  <si>
+    <t>Audit_time</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time when the audit was recorded</t>
   </si>
 </sst>
 </file>
@@ -456,7 +465,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -640,7 +649,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:F1"/>

</xml_diff>